<commit_message>
Codigo ajustado para agrupar lotes e vincular isso aos lotes antigos e remoção de HASH
</commit_message>
<xml_diff>
--- a/batch_grouping/new_datasets/lotes_agrupados.xlsx
+++ b/batch_grouping/new_datasets/lotes_agrupados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Lote ID</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -451,19 +451,24 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Qtd Agrupada</t>
+          <t>Quantidade</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>Lote_id</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>c4ca4238a0b923820dcc509a6f75849b</t>
+          <t>495223 Q2</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -477,16 +482,17 @@
       <c r="D2" t="n">
         <v>25</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>c81e728d9d4c2f636f067f89cc14862c</t>
+          <t>495223 Q2</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -500,16 +506,17 @@
       <c r="D3" t="n">
         <v>25</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>eccbc87e4b5ce2fe28308fd9f2a7baf3</t>
+          <t>495223 Q2</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -523,16 +530,17 @@
       <c r="D4" t="n">
         <v>25</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>a87ff679a2f3e71d9181a67b7542122c</t>
+          <t>495223 Q2</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -546,16 +554,17 @@
       <c r="D5" t="n">
         <v>20</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>e4da3b7fbbce2345d7772b0674a318d5</t>
+          <t>495223 Q3</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -569,16 +578,17 @@
       <c r="D6" t="n">
         <v>25</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1679091c5a880faf6fb5e6087eb1b2dc</t>
+          <t>495223 Q3</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -592,16 +602,17 @@
       <c r="D7" t="n">
         <v>25</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E7" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>8f14e45fceea167a5a36dedd4bea2543</t>
+          <t>495223 Q3</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -615,16 +626,17 @@
       <c r="D8" t="n">
         <v>2</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E8" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>c9f0f895fb98ab9159f51fd0297e236d</t>
+          <t>495224 Q1</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -638,16 +650,17 @@
       <c r="D9" t="n">
         <v>25</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>45c48cce2e2d7fbdea1afc51c7c6ad26</t>
+          <t>495224 Q3</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -661,16 +674,17 @@
       <c r="D10" t="n">
         <v>28</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E10" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>d3d9446802a44259755d38e6d163e820</t>
+          <t>495224 Q3</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -684,16 +698,17 @@
       <c r="D11" t="n">
         <v>16</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>6512bd43d9caa6e02c990b0a82652dca</t>
+          <t>495225 Q2</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -707,16 +722,17 @@
       <c r="D12" t="n">
         <v>30</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E12" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>c20ad4d76fe97759aa27a0c99bff6710</t>
+          <t>495225 Q2</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -730,16 +746,17 @@
       <c r="D13" t="n">
         <v>30</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E13" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>c51ce410c124a10e0db5e4b97fc2af39</t>
+          <t>495225 Q2</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -753,16 +770,17 @@
       <c r="D14" t="n">
         <v>30</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E14" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>aab3238922bcc25a6f606eb525ffdc56</t>
+          <t>495225 Q2</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -776,16 +794,17 @@
       <c r="D15" t="n">
         <v>30</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E15" t="n">
+        <v>14</v>
+      </c>
+      <c r="F15" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>9bf31c7ff062936a96d3c8bd1f8f2ff3</t>
+          <t>495225 Q3</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -793,22 +812,23 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Q2</t>
+          <t>Q3</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>17</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+        <v>30</v>
+      </c>
+      <c r="E16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>c74d97b01eae257e44aa9d5bade97baf</t>
+          <t>495225 Q3</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -820,41 +840,43 @@
         </is>
       </c>
       <c r="D17" t="n">
+        <v>11</v>
+      </c>
+      <c r="E17" t="n">
+        <v>16</v>
+      </c>
+      <c r="F17" t="n">
         <v>30</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>70efdf2ec9b086079795c442636b55fb</t>
+          <t>495226 Q1</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>495225</v>
+        <v>495226</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Q3</t>
+          <t>Q1</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>11</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+        <v>27</v>
+      </c>
+      <c r="E18" t="n">
+        <v>17</v>
+      </c>
+      <c r="F18" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>6f4922f45568161a8cdf4ad2299f6d23</t>
+          <t>495226 Q1</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -868,16 +890,17 @@
       <c r="D19" t="n">
         <v>27</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E19" t="n">
+        <v>18</v>
+      </c>
+      <c r="F19" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1f0e3dad99908345f7439f8ffabdffc4</t>
+          <t>495226 Q1</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -891,16 +914,17 @@
       <c r="D20" t="n">
         <v>27</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E20" t="n">
+        <v>19</v>
+      </c>
+      <c r="F20" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>98f13708210194c475687be6106a3b84</t>
+          <t>495226 Q1</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -912,18 +936,19 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>27</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="E21" t="n">
+        <v>20</v>
+      </c>
+      <c r="F21" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3c59dc048e8850243be8079a5c74d079</t>
+          <t>495226 Q2</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -931,22 +956,23 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>Q2</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+        <v>27</v>
+      </c>
+      <c r="E22" t="n">
+        <v>21</v>
+      </c>
+      <c r="F22" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>b6d767d2f8ed5d21a44b0e5886680cb9</t>
+          <t>495226 Q3</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -954,22 +980,23 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Q2</t>
+          <t>Q3</t>
         </is>
       </c>
       <c r="D23" t="n">
         <v>27</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="E23" t="n">
+        <v>22</v>
+      </c>
+      <c r="F23" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>37693cfc748049e45d87b8c7d8b9aacd</t>
+          <t>495226 Q3</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -977,22 +1004,23 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Q2</t>
+          <t>Q3</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>8</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+        <v>27</v>
+      </c>
+      <c r="E24" t="n">
+        <v>23</v>
+      </c>
+      <c r="F24" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1ff1de774005f8da13f42943881c655f</t>
+          <t>495226 Q3</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1004,22 +1032,23 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>27</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>24</v>
+      </c>
+      <c r="F25" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>8e296a067a37563370ded05f5a3bf3ec</t>
+          <t>495227 Q3</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>495226</v>
+        <v>495227</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1027,22 +1056,23 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>27</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+        <v>26</v>
+      </c>
+      <c r="E26" t="n">
+        <v>25</v>
+      </c>
+      <c r="F26" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4e732ced3463d06de0ca9a15b6153677</t>
+          <t>495227 Q3</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>495226</v>
+        <v>495227</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1050,58 +1080,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>5</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>02e74f10e0327ad868d138f2b4fdd6f0</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>495227</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Q3</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
+        <v>24</v>
+      </c>
+      <c r="E27" t="n">
         <v>26</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>33e75ff09dd601bbe69f351039152189</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>495227</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Q3</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>24</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Bloqueado</t>
-        </is>
+      <c r="F27" t="n">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>